<commit_message>
Aggiunti controlli che si specificano nella mail
</commit_message>
<xml_diff>
--- a/CDR_CE_LT068_GSM_MODERNIZATION_ver1.xlsx
+++ b/CDR_CE_LT068_GSM_MODERNIZATION_ver1.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D143CF6-0BA9-41F1-8C8D-DE51CD37D9B8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAD8A098-2883-45BF-AE23-B9FB3288F51D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6855" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3434,7 +3434,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E4" sqref="E4"/>
+      <selection pane="topRight" activeCell="H3" sqref="H2:H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3605,14 +3605,14 @@
         <v>102</v>
       </c>
       <c r="F2" s="38">
-        <v>34561</v>
+        <v>34562</v>
       </c>
       <c r="G2" s="31">
         <v>52404</v>
       </c>
       <c r="H2" s="15" t="str">
-        <f t="shared" ref="H2:H6" si="1">"222-88-"&amp;F2&amp;"-"&amp;G2</f>
-        <v>222-88-34561-52404</v>
+        <f>"222-88-"&amp;F2&amp;"-"&amp;G2</f>
+        <v>222-88-34562-52404</v>
       </c>
       <c r="I2" s="2">
         <v>7</v>
@@ -3639,26 +3639,26 @@
         <v>43</v>
       </c>
       <c r="Q2" s="15">
-        <f t="shared" ref="Q2:Q6" si="2">P2</f>
+        <f t="shared" ref="Q2:Q6" si="1">P2</f>
         <v>43</v>
       </c>
       <c r="R2" s="31">
         <v>56</v>
       </c>
       <c r="S2" s="15">
-        <f t="shared" ref="S2:S6" si="3">R2</f>
+        <f t="shared" ref="S2:S6" si="2">R2</f>
         <v>56</v>
       </c>
       <c r="T2" s="15">
-        <f t="shared" ref="T2:T6" si="4">IF(MID(C2,6,1)="G",104,IF(MID(C2,6,1)="D",102,"NA"))</f>
+        <f t="shared" ref="T2:T6" si="3">IF(MID(C2,6,1)="G",104,IF(MID(C2,6,1)="D",102,"NA"))</f>
         <v>104</v>
       </c>
       <c r="U2" s="15">
-        <f t="shared" ref="U2:U6" si="5">IF(MID(C2,6,1)="G",33,IF(MID(C2,6,1)="D",30,"NA"))</f>
+        <f t="shared" ref="U2:U6" si="4">IF(MID(C2,6,1)="G",33,IF(MID(C2,6,1)="D",30,"NA"))</f>
         <v>33</v>
       </c>
       <c r="V2" s="15">
-        <f t="shared" ref="V2:V6" si="6">U2</f>
+        <f t="shared" ref="V2:V6" si="5">U2</f>
         <v>33</v>
       </c>
       <c r="W2" s="15">
@@ -3673,11 +3673,11 @@
         <v>SY</v>
       </c>
       <c r="Z2" s="15">
-        <f t="shared" ref="Z2:Z6" si="7">IF(AA2&gt;16,1,0)</f>
+        <f t="shared" ref="Z2:Z6" si="6">IF(AA2&gt;16,1,0)</f>
         <v>0</v>
       </c>
       <c r="AA2" s="15">
-        <f t="shared" ref="AA2:AA6" si="8">8*X2</f>
+        <f t="shared" ref="AA2:AA6" si="7">8*X2</f>
         <v>8</v>
       </c>
       <c r="AB2" s="38">
@@ -3724,7 +3724,7 @@
         <v>52405</v>
       </c>
       <c r="H3" s="15" t="str">
-        <f t="shared" si="1"/>
+        <f>"222-88-"&amp;F3&amp;"-"&amp;G3</f>
         <v>222-88-34561-52405</v>
       </c>
       <c r="I3" s="2">
@@ -3752,45 +3752,45 @@
         <v>43</v>
       </c>
       <c r="Q3" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>43</v>
       </c>
       <c r="R3" s="31">
         <v>56</v>
       </c>
       <c r="S3" s="15">
+        <f t="shared" si="2"/>
+        <v>56</v>
+      </c>
+      <c r="T3" s="15">
         <f t="shared" si="3"/>
-        <v>56</v>
-      </c>
-      <c r="T3" s="15">
+        <v>104</v>
+      </c>
+      <c r="U3" s="15">
         <f t="shared" si="4"/>
-        <v>104</v>
-      </c>
-      <c r="U3" s="15">
+        <v>33</v>
+      </c>
+      <c r="V3" s="15">
         <f t="shared" si="5"/>
         <v>33</v>
       </c>
-      <c r="V3" s="15">
-        <f t="shared" si="6"/>
-        <v>33</v>
-      </c>
       <c r="W3" s="15">
-        <f t="shared" ref="W3:W6" si="9">IF(X3&lt;&gt;"",1,"")</f>
+        <f t="shared" ref="W3:W6" si="8">IF(X3&lt;&gt;"",1,"")</f>
         <v>1</v>
       </c>
       <c r="X3" s="31">
         <v>2</v>
       </c>
       <c r="Y3" s="15" t="str">
-        <f t="shared" ref="Y3:Y6" si="10">IF(X3&lt;&gt;"","SY","")</f>
+        <f t="shared" ref="Y3:Y6" si="9">IF(X3&lt;&gt;"","SY","")</f>
         <v>SY</v>
       </c>
       <c r="Z3" s="15">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AA3" s="15">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="AA3" s="15">
-        <f t="shared" si="8"/>
         <v>16</v>
       </c>
       <c r="AB3" s="38">
@@ -3837,7 +3837,7 @@
         <v>52406</v>
       </c>
       <c r="H4" s="15" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="H2:H6" si="10">"222-88-"&amp;F4&amp;"-"&amp;G4</f>
         <v>222-88-34561-52406</v>
       </c>
       <c r="I4" s="2">
@@ -3865,45 +3865,45 @@
         <v>43</v>
       </c>
       <c r="Q4" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>43</v>
       </c>
       <c r="R4" s="31">
         <v>56</v>
       </c>
       <c r="S4" s="15">
+        <f t="shared" si="2"/>
+        <v>56</v>
+      </c>
+      <c r="T4" s="15">
         <f t="shared" si="3"/>
-        <v>56</v>
-      </c>
-      <c r="T4" s="15">
+        <v>104</v>
+      </c>
+      <c r="U4" s="15">
         <f t="shared" si="4"/>
-        <v>104</v>
-      </c>
-      <c r="U4" s="15">
+        <v>33</v>
+      </c>
+      <c r="V4" s="15">
         <f t="shared" si="5"/>
         <v>33</v>
       </c>
-      <c r="V4" s="15">
-        <f t="shared" si="6"/>
-        <v>33</v>
-      </c>
       <c r="W4" s="15">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="X4" s="31">
         <v>2</v>
       </c>
       <c r="Y4" s="15" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>SY</v>
       </c>
       <c r="Z4" s="15">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AA4" s="15">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="AA4" s="15">
-        <f t="shared" si="8"/>
         <v>16</v>
       </c>
       <c r="AB4" s="38">
@@ -3950,7 +3950,7 @@
         <v>64465</v>
       </c>
       <c r="H5" s="15" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="10"/>
         <v>222-88-34561-64465</v>
       </c>
       <c r="I5" s="2">
@@ -3978,45 +3978,45 @@
         <v>43</v>
       </c>
       <c r="Q5" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>43</v>
       </c>
       <c r="R5" s="31">
         <v>56</v>
       </c>
       <c r="S5" s="15">
+        <f t="shared" si="2"/>
+        <v>56</v>
+      </c>
+      <c r="T5" s="15">
         <f t="shared" si="3"/>
-        <v>56</v>
-      </c>
-      <c r="T5" s="15">
+        <v>102</v>
+      </c>
+      <c r="U5" s="15">
         <f t="shared" si="4"/>
-        <v>102</v>
-      </c>
-      <c r="U5" s="15">
+        <v>30</v>
+      </c>
+      <c r="V5" s="15">
         <f t="shared" si="5"/>
         <v>30</v>
       </c>
-      <c r="V5" s="15">
-        <f t="shared" si="6"/>
-        <v>30</v>
-      </c>
       <c r="W5" s="15">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="X5" s="31">
         <v>3</v>
       </c>
       <c r="Y5" s="15" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>SY</v>
       </c>
       <c r="Z5" s="15">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="AA5" s="15">
         <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="AA5" s="15">
-        <f t="shared" si="8"/>
         <v>24</v>
       </c>
       <c r="AB5" s="31">
@@ -4071,7 +4071,7 @@
         <v>64466</v>
       </c>
       <c r="H6" s="15" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="10"/>
         <v>222-88-34561-64466</v>
       </c>
       <c r="I6" s="2">
@@ -4099,45 +4099,45 @@
         <v>43</v>
       </c>
       <c r="Q6" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>43</v>
       </c>
       <c r="R6" s="31">
         <v>56</v>
       </c>
       <c r="S6" s="15">
+        <f t="shared" si="2"/>
+        <v>56</v>
+      </c>
+      <c r="T6" s="15">
         <f t="shared" si="3"/>
-        <v>56</v>
-      </c>
-      <c r="T6" s="15">
+        <v>102</v>
+      </c>
+      <c r="U6" s="15">
         <f t="shared" si="4"/>
-        <v>102</v>
-      </c>
-      <c r="U6" s="15">
+        <v>30</v>
+      </c>
+      <c r="V6" s="15">
         <f t="shared" si="5"/>
         <v>30</v>
       </c>
-      <c r="V6" s="15">
-        <f t="shared" si="6"/>
-        <v>30</v>
-      </c>
       <c r="W6" s="15">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="X6" s="31">
         <v>3</v>
       </c>
       <c r="Y6" s="15" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>SY</v>
       </c>
       <c r="Z6" s="15">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="AA6" s="15">
         <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="AA6" s="15">
-        <f t="shared" si="8"/>
         <v>24</v>
       </c>
       <c r="AB6" s="31">

</xml_diff>

<commit_message>
Creazione eseguibile e implementazione regole e miglioramento gui
</commit_message>
<xml_diff>
--- a/CDR_CE_LT068_GSM_MODERNIZATION_ver1.xlsx
+++ b/CDR_CE_LT068_GSM_MODERNIZATION_ver1.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{282EAC29-C090-44C5-B192-947D7515B69A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{792292FA-361D-48BB-966B-1591DAC44CE0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6855" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1178,7 +1178,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="111">
   <si>
     <t>TG</t>
   </si>
@@ -1486,9 +1486,6 @@
     <t>RM01BSC</t>
   </si>
   <si>
-    <t>RXSTG-456</t>
-  </si>
-  <si>
     <t>RXSTG-458</t>
   </si>
   <si>
@@ -1513,7 +1510,7 @@
     <t>R1</t>
   </si>
   <si>
-    <t>222-88-34562-52404</t>
+    <t>RXSTG-457</t>
   </si>
 </sst>
 </file>
@@ -2705,7 +2702,7 @@
     <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2797,9 +2794,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="56" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="56" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="261">
     <cellStyle name="_x000a_shell=progma" xfId="4" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -3437,8 +3431,7 @@
   <dimension ref="A1:AL15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="3" topLeftCell="E1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H3" sqref="H3"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3606,7 +3599,7 @@
         <v>LT068G</v>
       </c>
       <c r="E2" s="31" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="F2" s="38">
         <v>34562</v>
@@ -3718,8 +3711,8 @@
         <f t="shared" si="0"/>
         <v>LT068G</v>
       </c>
-      <c r="E3" s="41" t="s">
-        <v>102</v>
+      <c r="E3" s="31" t="s">
+        <v>110</v>
       </c>
       <c r="F3" s="38">
         <v>34561</v>
@@ -3727,8 +3720,9 @@
       <c r="G3" s="31">
         <v>52405</v>
       </c>
-      <c r="H3" s="15" t="s">
-        <v>111</v>
+      <c r="H3" s="15" t="str">
+        <f>"222-88-"&amp;F3&amp;"-"&amp;G3</f>
+        <v>222-88-34561-52405</v>
       </c>
       <c r="I3" s="2">
         <v>7</v>
@@ -3833,7 +3827,7 @@
         <v>LT068G</v>
       </c>
       <c r="E4" s="31" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F4" s="38">
         <v>34561</v>
@@ -3948,7 +3942,7 @@
         <v>LT068D</v>
       </c>
       <c r="E5" s="31" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F5" s="38">
         <v>34561</v>
@@ -4069,7 +4063,7 @@
         <v>LT068D</v>
       </c>
       <c r="E6" s="31" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F6" s="38">
         <v>34561</v>
@@ -4254,7 +4248,7 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="28" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B2" s="16" t="str">
         <f>[1]BTS!$B$2</f>
@@ -4284,7 +4278,7 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="28" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B3" s="16" t="str">
         <f>[1]BTS!$B$2</f>
@@ -4314,7 +4308,7 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="28" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B4" s="16" t="str">
         <f>[1]BTS!$B$2</f>
@@ -4344,7 +4338,7 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="28" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B5" s="16" t="str">
         <f>[1]BTS!$B$2</f>
@@ -4374,7 +4368,7 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="28" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B6" s="16" t="str">
         <f>[1]BTS!$B$2</f>
@@ -4404,7 +4398,7 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="28" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B7" s="16" t="str">
         <f>[1]BTS!$B$2</f>
@@ -4434,7 +4428,7 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="28" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B8" s="16" t="str">
         <f>[1]BTS!$B$2</f>
@@ -4464,7 +4458,7 @@
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="28" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B9" s="16" t="str">
         <f>[1]BTS!$B$2</f>
@@ -4494,7 +4488,7 @@
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="28" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B10" s="16" t="str">
         <f>[1]BTS!$B$2</f>
@@ -4524,7 +4518,7 @@
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="28" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B11" s="16" t="str">
         <f>[1]BTS!$B$2</f>
@@ -4554,7 +4548,7 @@
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="28" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B12" s="16" t="str">
         <f>[1]BTS!$B$2</f>
@@ -4584,7 +4578,7 @@
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="28" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B13" s="16" t="str">
         <f>[1]BTS!$B$2</f>
@@ -4614,7 +4608,7 @@
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="28" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B14" s="16" t="str">
         <f>[1]BTS!$B$2</f>
@@ -4644,7 +4638,7 @@
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="28" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B15" s="16" t="str">
         <f>[1]BTS!$B$2</f>
@@ -4674,7 +4668,7 @@
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="28" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B16" s="16" t="str">
         <f>[1]BTS!$B$2</f>
@@ -4704,7 +4698,7 @@
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="28" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B17" s="16" t="str">
         <f>[1]BTS!$B$2</f>
@@ -4734,7 +4728,7 @@
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="28" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B18" s="16" t="str">
         <f>[1]BTS!$B$2</f>
@@ -4764,7 +4758,7 @@
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="28" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B19" s="16" t="str">
         <f>[1]BTS!$B$2</f>
@@ -4794,7 +4788,7 @@
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="28" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B20" s="16" t="str">
         <f>[1]BTS!$B$2</f>
@@ -4824,7 +4818,7 @@
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="28" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B21" s="16" t="str">
         <f>[1]BTS!$B$2</f>
@@ -4901,7 +4895,7 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="28" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B2" s="34" t="str">
         <f>[1]BTS!$B$2</f>
@@ -4927,7 +4921,7 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="28" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B3" s="34" t="str">
         <f>[1]BTS!$B$2</f>
@@ -4953,7 +4947,7 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="28" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B4" s="34" t="str">
         <f>[1]BTS!$B$2</f>
@@ -4979,7 +4973,7 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="28" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B5" s="34" t="str">
         <f>[1]BTS!$B$2</f>
@@ -5005,7 +4999,7 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="28" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B6" s="34" t="str">
         <f>[1]BTS!$B$2</f>
@@ -5031,7 +5025,7 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="28" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B7" s="34" t="str">
         <f>[1]BTS!$B$2</f>
@@ -5057,7 +5051,7 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="28" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B8" s="34" t="str">
         <f>[1]BTS!$B$2</f>
@@ -5083,7 +5077,7 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="28" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B9" s="34" t="str">
         <f>[1]BTS!$B$2</f>
@@ -5109,7 +5103,7 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="28" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B10" s="34" t="str">
         <f>[1]BTS!$B$2</f>
@@ -5135,7 +5129,7 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="28" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B11" s="34" t="str">
         <f>[1]BTS!$B$2</f>
@@ -5161,7 +5155,7 @@
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="28" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B12" s="34" t="str">
         <f>[1]BTS!$B$2</f>
@@ -5187,7 +5181,7 @@
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="28" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B13" s="34" t="str">
         <f>[1]BTS!$B$2</f>
@@ -5213,7 +5207,7 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="28" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B14" s="34" t="str">
         <f>[1]BTS!$B$2</f>
@@ -5239,7 +5233,7 @@
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="28" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B15" s="34" t="str">
         <f>[1]BTS!$B$2</f>
@@ -5265,7 +5259,7 @@
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="28" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B16" s="34" t="str">
         <f>[1]BTS!$B$2</f>
@@ -5291,7 +5285,7 @@
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="28" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B17" s="34" t="str">
         <f>[1]BTS!$B$2</f>
@@ -5312,12 +5306,12 @@
         <v>73</v>
       </c>
       <c r="G17" s="33" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="28" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B18" s="34" t="str">
         <f>[1]BTS!$B$2</f>
@@ -5338,12 +5332,12 @@
         <v>73</v>
       </c>
       <c r="G18" s="33" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="28" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B19" s="34" t="str">
         <f>[1]BTS!$B$2</f>
@@ -5364,12 +5358,12 @@
         <v>73</v>
       </c>
       <c r="G19" s="33" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="28" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B20" s="34" t="str">
         <f>[1]BTS!$B$2</f>
@@ -5395,7 +5389,7 @@
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="28" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B21" s="34" t="str">
         <f>[1]BTS!$B$2</f>
@@ -5421,7 +5415,7 @@
     </row>
     <row r="22" spans="1:7">
       <c r="A22" s="28" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B22" s="34" t="str">
         <f>[1]BTS!$B$2</f>
@@ -5447,7 +5441,7 @@
     </row>
     <row r="23" spans="1:7">
       <c r="A23" s="28" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B23" s="34" t="str">
         <f>[1]BTS!$B$2</f>
@@ -5473,7 +5467,7 @@
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="28" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B24" s="34" t="str">
         <f>[1]BTS!$B$2</f>
@@ -5499,7 +5493,7 @@
     </row>
     <row r="25" spans="1:7">
       <c r="A25" s="28" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B25" s="34" t="str">
         <f>[1]BTS!$B$2</f>
@@ -5525,7 +5519,7 @@
     </row>
     <row r="26" spans="1:7">
       <c r="A26" s="28" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B26" s="34" t="str">
         <f>[1]BTS!$B$2</f>
@@ -5551,7 +5545,7 @@
     </row>
     <row r="27" spans="1:7">
       <c r="A27" s="28" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B27" s="34" t="str">
         <f>[1]BTS!$B$2</f>
@@ -5577,7 +5571,7 @@
     </row>
     <row r="28" spans="1:7">
       <c r="A28" s="28" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B28" s="34" t="str">
         <f>[1]BTS!$B$2</f>
@@ -5603,7 +5597,7 @@
     </row>
     <row r="29" spans="1:7">
       <c r="A29" s="28" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B29" s="34" t="str">
         <f>[1]BTS!$B$2</f>
@@ -5629,7 +5623,7 @@
     </row>
     <row r="30" spans="1:7">
       <c r="A30" s="28" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B30" s="34" t="str">
         <f>[1]BTS!$B$2</f>
@@ -5655,7 +5649,7 @@
     </row>
     <row r="31" spans="1:7">
       <c r="A31" s="28" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B31" s="34" t="str">
         <f>[1]BTS!$B$2</f>
@@ -5778,7 +5772,7 @@
         <v>LT068R1</v>
       </c>
       <c r="C2" s="28" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D2" s="28">
         <v>402</v>
@@ -5847,7 +5841,7 @@
         <v>LT068R2</v>
       </c>
       <c r="C3" s="28" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D3" s="28">
         <v>402</v>
@@ -5916,7 +5910,7 @@
         <v>LT068R3</v>
       </c>
       <c r="C4" s="28" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D4" s="28">
         <v>402</v>
@@ -5985,7 +5979,7 @@
         <v>LT068U1</v>
       </c>
       <c r="C5" s="28" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D5" s="28">
         <v>402</v>
@@ -6054,7 +6048,7 @@
         <v>LT068U2</v>
       </c>
       <c r="C6" s="28" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D6" s="28">
         <v>402</v>
@@ -6123,7 +6117,7 @@
         <v>LT068U3</v>
       </c>
       <c r="C7" s="28" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D7" s="28">
         <v>402</v>
@@ -6192,7 +6186,7 @@
         <v>LT068V1</v>
       </c>
       <c r="C8" s="28" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D8" s="28">
         <v>402</v>
@@ -6261,7 +6255,7 @@
         <v>LT068V2</v>
       </c>
       <c r="C9" s="28" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D9" s="28">
         <v>402</v>
@@ -6330,7 +6324,7 @@
         <v>LT068V3</v>
       </c>
       <c r="C10" s="28" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D10" s="28">
         <v>402</v>
@@ -6399,7 +6393,7 @@
         <v>LT068W1</v>
       </c>
       <c r="C11" s="28" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D11" s="28">
         <v>402</v>
@@ -6468,7 +6462,7 @@
         <v>LT068W2</v>
       </c>
       <c r="C12" s="28" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D12" s="28">
         <v>402</v>
@@ -6537,7 +6531,7 @@
         <v>LT068W3</v>
       </c>
       <c r="C13" s="28" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D13" s="28">
         <v>402</v>

</xml_diff>

<commit_message>
Creato exe, agiunti altri controlli, agggiunta funzionalità di poter visualizzare la cartella del file error
</commit_message>
<xml_diff>
--- a/CDR_CE_LT068_GSM_MODERNIZATION_ver1.xlsx
+++ b/CDR_CE_LT068_GSM_MODERNIZATION_ver1.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{792292FA-361D-48BB-966B-1591DAC44CE0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B1136E6-358B-46D8-A863-DB82EFDAF99E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6855" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1178,7 +1178,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="112">
   <si>
     <t>TG</t>
   </si>
@@ -1511,6 +1511,9 @@
   </si>
   <si>
     <t>RXSTG-457</t>
+  </si>
+  <si>
+    <t>RXSTG-456</t>
   </si>
 </sst>
 </file>
@@ -2702,7 +2705,7 @@
     <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2794,6 +2797,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="56" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="56" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="261">
     <cellStyle name="_x000a_shell=progma" xfId="4" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -3431,7 +3435,7 @@
   <dimension ref="A1:AL15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3599,7 +3603,7 @@
         <v>LT068G</v>
       </c>
       <c r="E2" s="31" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F2" s="38">
         <v>34562</v>
@@ -3796,7 +3800,9 @@
       <c r="AC3" s="31">
         <v>0</v>
       </c>
-      <c r="AD3" s="31"/>
+      <c r="AD3" s="31">
+        <v>1</v>
+      </c>
       <c r="AE3" s="31"/>
       <c r="AF3" s="31">
         <v>120</v>
@@ -3911,7 +3917,9 @@
       <c r="AC4" s="31">
         <v>1</v>
       </c>
-      <c r="AD4" s="31"/>
+      <c r="AD4" s="31">
+        <v>1</v>
+      </c>
       <c r="AE4" s="31"/>
       <c r="AF4" s="31">
         <v>102</v>
@@ -4052,7 +4060,7 @@
       <c r="A6" s="35" t="s">
         <v>70</v>
       </c>
-      <c r="B6" s="30" t="s">
+      <c r="B6" s="41" t="s">
         <v>101</v>
       </c>
       <c r="C6" s="31" t="s">

</xml_diff>

<commit_message>
agg. Regola per controllo su frequenze e bug fix
</commit_message>
<xml_diff>
--- a/CDR_CE_LT068_GSM_MODERNIZATION_ver1.xlsx
+++ b/CDR_CE_LT068_GSM_MODERNIZATION_ver1.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B1136E6-358B-46D8-A863-DB82EFDAF99E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0BA1BFA-09E3-44DC-B403-CB8CCF42D057}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6855" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2705,7 +2705,7 @@
     <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2798,6 +2798,7 @@
     <xf numFmtId="0" fontId="0" fillId="56" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="56" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="56" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="261">
     <cellStyle name="_x000a_shell=progma" xfId="4" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -3434,8 +3435,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AL15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3449,23 +3450,24 @@
     <col min="8" max="8" width="22" customWidth="1"/>
     <col min="10" max="10" width="12.7109375" customWidth="1"/>
     <col min="11" max="11" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="28.42578125" style="26" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="22.140625" style="26" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="22.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18.42578125" customWidth="1"/>
-    <col min="17" max="17" width="18.28515625" customWidth="1"/>
-    <col min="18" max="18" width="14.5703125" style="26" customWidth="1"/>
-    <col min="19" max="19" width="17.5703125" style="26" customWidth="1"/>
-    <col min="20" max="22" width="18.28515625" style="3" customWidth="1"/>
-    <col min="23" max="23" width="28.42578125" style="26" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="28.42578125" style="26" customWidth="1"/>
-    <col min="25" max="25" width="16.85546875" style="26" customWidth="1"/>
-    <col min="26" max="26" width="22.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="28.42578125" style="26" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="22.140625" style="26" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="22.42578125" style="3" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="17.7109375" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="18.42578125" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="18.28515625" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="14.5703125" style="26" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="17.5703125" style="26" hidden="1" customWidth="1"/>
+    <col min="20" max="22" width="18.28515625" style="3" hidden="1" customWidth="1"/>
+    <col min="23" max="23" width="28.42578125" style="26" hidden="1" customWidth="1"/>
+    <col min="24" max="24" width="21.5703125" style="26" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="6.28515625" style="26" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="16.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="17.7109375" customWidth="1"/>
-    <col min="29" max="29" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="30" max="31" width="23.42578125" style="26" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="17.7109375" style="26" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="35.5703125" style="26" customWidth="1"/>
     <col min="32" max="35" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="19.7109375" customWidth="1"/>
     <col min="37" max="37" width="20.28515625" customWidth="1"/>
@@ -3689,16 +3691,16 @@
       </c>
       <c r="AD2" s="31"/>
       <c r="AE2" s="31"/>
-      <c r="AF2" s="31">
+      <c r="AF2" s="42">
         <v>100</v>
       </c>
-      <c r="AG2" s="31">
+      <c r="AG2" s="42">
         <v>104</v>
       </c>
-      <c r="AH2" s="30"/>
-      <c r="AI2" s="30"/>
-      <c r="AJ2" s="30"/>
-      <c r="AK2" s="30"/>
+      <c r="AH2" s="42"/>
+      <c r="AI2" s="42"/>
+      <c r="AJ2" s="42"/>
+      <c r="AK2" s="42"/>
       <c r="AL2" s="30"/>
     </row>
     <row r="3" spans="1:38" s="5" customFormat="1" ht="15.75" customHeight="1">
@@ -3804,18 +3806,18 @@
         <v>1</v>
       </c>
       <c r="AE3" s="31"/>
-      <c r="AF3" s="31">
+      <c r="AF3" s="42">
         <v>120</v>
       </c>
-      <c r="AG3" s="31">
+      <c r="AG3" s="42">
         <v>124</v>
       </c>
-      <c r="AH3" s="31">
+      <c r="AH3" s="42">
         <v>124</v>
       </c>
-      <c r="AI3" s="30"/>
-      <c r="AJ3" s="30"/>
-      <c r="AK3" s="30"/>
+      <c r="AI3" s="42"/>
+      <c r="AJ3" s="42"/>
+      <c r="AK3" s="42"/>
       <c r="AL3" s="30"/>
     </row>
     <row r="4" spans="1:38" s="5" customFormat="1">
@@ -3921,18 +3923,18 @@
         <v>1</v>
       </c>
       <c r="AE4" s="31"/>
-      <c r="AF4" s="31">
+      <c r="AF4" s="42">
         <v>102</v>
       </c>
-      <c r="AG4" s="31">
+      <c r="AG4" s="42">
         <v>121</v>
       </c>
-      <c r="AH4" s="31">
+      <c r="AH4" s="42">
         <v>121</v>
       </c>
-      <c r="AI4" s="30"/>
-      <c r="AJ4" s="30"/>
-      <c r="AK4" s="30"/>
+      <c r="AI4" s="42"/>
+      <c r="AJ4" s="42"/>
+      <c r="AK4" s="42"/>
       <c r="AL4" s="30"/>
     </row>
     <row r="5" spans="1:38" s="5" customFormat="1">
@@ -4040,20 +4042,20 @@
       <c r="AE5" s="31">
         <v>1</v>
       </c>
-      <c r="AF5" s="31">
+      <c r="AF5" s="42">
         <v>693</v>
       </c>
-      <c r="AG5" s="31">
+      <c r="AG5" s="42">
         <v>696</v>
       </c>
-      <c r="AH5" s="30">
+      <c r="AH5" s="42">
         <v>702</v>
       </c>
-      <c r="AI5" s="30">
+      <c r="AI5" s="42">
         <v>700</v>
       </c>
-      <c r="AJ5" s="30"/>
-      <c r="AK5" s="30"/>
+      <c r="AJ5" s="42"/>
+      <c r="AK5" s="42"/>
       <c r="AL5" s="30"/>
     </row>
     <row r="6" spans="1:38" s="5" customFormat="1">
@@ -4161,20 +4163,20 @@
       <c r="AE6" s="31">
         <v>0</v>
       </c>
-      <c r="AF6" s="31">
+      <c r="AF6" s="42">
         <v>695</v>
       </c>
-      <c r="AG6" s="31">
+      <c r="AG6" s="42">
         <v>688</v>
       </c>
-      <c r="AH6" s="30">
+      <c r="AH6" s="42">
         <v>689</v>
       </c>
-      <c r="AI6" s="30">
+      <c r="AI6" s="42">
         <v>701</v>
       </c>
-      <c r="AJ6" s="30"/>
-      <c r="AK6" s="30"/>
+      <c r="AJ6" s="42"/>
+      <c r="AK6" s="42"/>
       <c r="AL6" s="30"/>
     </row>
     <row r="7" spans="1:38">
@@ -4869,7 +4871,7 @@
   <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A8" sqref="A7:A8"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Creazione exe con nuova interfaccia; Commenti per i vari controlli; Tolti alcuni bug;
</commit_message>
<xml_diff>
--- a/CDR_CE_LT068_GSM_MODERNIZATION_ver1.xlsx
+++ b/CDR_CE_LT068_GSM_MODERNIZATION_ver1.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1"/>
+  <workbookPr filterPrivacy="1" codeName="Questa_cartella_di_lavoro"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6855" activeTab="1"/>
   </bookViews>
@@ -23,7 +23,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">BTS!$B$1:$AL$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'External 3G cells'!$A$1:$U$13</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -3370,6 +3370,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Foglio1"/>
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3432,45 +3433,47 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Foglio2"/>
   <dimension ref="A1:AL15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AB1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="AH4" sqref="AH4"/>
+    <sheetView tabSelected="1" topLeftCell="R1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="AB2" sqref="AB2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" customWidth="1"/>
-    <col min="6" max="7" width="15.42578125" style="3" customWidth="1"/>
-    <col min="8" max="8" width="22" customWidth="1"/>
-    <col min="10" max="10" width="12.7109375" customWidth="1"/>
-    <col min="11" max="11" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="28.42578125" style="26" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="22.140625" style="26" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="22.42578125" style="3" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="17.7109375" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="18.42578125" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="18.28515625" hidden="1" customWidth="1"/>
-    <col min="18" max="18" width="14.5703125" style="26" hidden="1" customWidth="1"/>
-    <col min="19" max="19" width="17.5703125" style="26" hidden="1" customWidth="1"/>
-    <col min="20" max="22" width="18.28515625" style="3" hidden="1" customWidth="1"/>
-    <col min="23" max="23" width="28.42578125" style="26" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.7109375" style="26" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.42578125" style="26" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="22.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7.85546875" style="26" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.140625" style="26" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="22.7109375" style="26" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="21.5703125" style="26" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="6.28515625" style="26" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="16.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="22.28515625" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="17.7109375" style="26" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="35.5703125" style="26" customWidth="1"/>
-    <col min="32" max="35" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="19.7109375" customWidth="1"/>
-    <col min="37" max="37" width="20.28515625" customWidth="1"/>
-    <col min="38" max="38" width="26.7109375" customWidth="1"/>
+    <col min="30" max="31" width="17.7109375" style="26" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="19.42578125" customWidth="1"/>
+    <col min="33" max="37" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="18.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:38" s="14" customFormat="1">
@@ -3683,15 +3686,15 @@
         <v>8</v>
       </c>
       <c r="AB2" s="38">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="AC2" s="31">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="AD2" s="31"/>
       <c r="AE2" s="31"/>
       <c r="AF2" s="42">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="AG2" s="42">
         <v>104</v>
@@ -3704,7 +3707,7 @@
       <c r="AK2" s="42"/>
       <c r="AL2" s="30"/>
     </row>
-    <row r="3" spans="1:38" s="5" customFormat="1" ht="15.75" customHeight="1">
+    <row r="3" spans="1:38" s="5" customFormat="1">
       <c r="A3" s="35" t="s">
         <v>70</v>
       </c>
@@ -3801,10 +3804,10 @@
         <v>6</v>
       </c>
       <c r="AC3" s="31">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AD3" s="31">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="AE3" s="31"/>
       <c r="AF3" s="42">
@@ -3921,7 +3924,7 @@
         <v>1</v>
       </c>
       <c r="AD4" s="31">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="AE4" s="31"/>
       <c r="AF4" s="42">
@@ -4035,7 +4038,7 @@
         <v>4</v>
       </c>
       <c r="AC5" s="31">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AD5" s="31">
         <v>2</v>
@@ -4053,7 +4056,7 @@
         <v>702</v>
       </c>
       <c r="AI5" s="42">
-        <v>700</v>
+        <v>800</v>
       </c>
       <c r="AJ5" s="42"/>
       <c r="AK5" s="42"/>
@@ -4159,7 +4162,7 @@
         <v>2</v>
       </c>
       <c r="AD6" s="31">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="AE6" s="31">
         <v>0</v>
@@ -4220,6 +4223,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Foglio3"/>
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4869,6 +4873,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Foglio4"/>
   <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
@@ -5693,6 +5698,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Foglio5"/>
   <dimension ref="A1:U13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6614,6 +6620,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Foglio6"/>
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>